<commit_message>
Fixed problem with copying
</commit_message>
<xml_diff>
--- a/datasets/data4.xlsx
+++ b/datasets/data4.xlsx
@@ -506,7 +506,7 @@
       <selection activeCell="F380" sqref="F380"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.7109375" customWidth="1" min="5" max="5"/>
   </cols>
@@ -618,6 +618,11 @@
           <t>Director</t>
         </is>
       </c>
+      <c r="E4" s="11" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">

</xml_diff>